<commit_message>
Added lab3 data summary
</commit_message>
<xml_diff>
--- a/Lab3/lab3 data summary.xlsx
+++ b/Lab3/lab3 data summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Visibilities PLot" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
   <si>
     <t>File</t>
   </si>
@@ -179,51 +178,9 @@
     <t>Filename</t>
   </si>
   <si>
-    <t>Pmax (1st order)</t>
-  </si>
-  <si>
-    <t>Pmin (1st order)</t>
-  </si>
-  <si>
-    <t>Pmax (2nd order)</t>
-  </si>
-  <si>
-    <t>Pmin (2nd order)</t>
-  </si>
-  <si>
-    <t>Pmin (3rd order)</t>
-  </si>
-  <si>
-    <t>Pmax (3rd order)</t>
-  </si>
-  <si>
-    <t>Visibility (avg)</t>
-  </si>
-  <si>
     <t>sun_inter_18</t>
   </si>
   <si>
-    <t>Visibility (1st)</t>
-  </si>
-  <si>
-    <t>Visibility (2nd)</t>
-  </si>
-  <si>
-    <t>Visibility (3rd)</t>
-  </si>
-  <si>
-    <t>Pmax 4</t>
-  </si>
-  <si>
-    <t>Pmin 4</t>
-  </si>
-  <si>
-    <t>Visibility (4)</t>
-  </si>
-  <si>
-    <t>Visibility (std dev)</t>
-  </si>
-  <si>
     <t>sun_inter_20</t>
   </si>
   <si>
@@ -264,6 +221,33 @@
   </si>
   <si>
     <t>Visibility (error)</t>
+  </si>
+  <si>
+    <t>Lambda/B</t>
+  </si>
+  <si>
+    <t>Baseline 1</t>
+  </si>
+  <si>
+    <t>Baseline 2</t>
+  </si>
+  <si>
+    <t>Baseline 3</t>
+  </si>
+  <si>
+    <t>Baseline 4</t>
+  </si>
+  <si>
+    <t>Baseline (avg)</t>
+  </si>
+  <si>
+    <t>Baseline (std dev)</t>
+  </si>
+  <si>
+    <t>Baseline (cm)</t>
+  </si>
+  <si>
+    <t>Correction (cosine of altitude)</t>
   </si>
 </sst>
 </file>
@@ -318,6 +302,961 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Visibilities PLot'!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Visibilities PLot'!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.21587308408976721</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21297288998783143</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15365832338361227</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19553991597284306</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16166065213986197</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18844435666384207</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.223006203619358</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28014465417666967</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18772020190913313</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15669573473540771</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.19982384896693572</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.7935319202984288E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.4832432703516743E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AED2-4342-B8C6-7BF8C568C506}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="478503648"/>
+        <c:axId val="478507256"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="478503648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="478507256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="478507256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="478503648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04E89DFB-56C0-4A56-8B34-62738C5628E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -619,8 +1558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,6 +1631,9 @@
       <c r="F3" s="1">
         <v>0.45208333333333334</v>
       </c>
+      <c r="G3" s="2">
+        <v>1.875</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1424,797 +2366,634 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2">
+        <v>76.2</v>
+      </c>
+      <c r="C2">
+        <v>2.2689277000000001E-2</v>
+      </c>
+      <c r="D2">
+        <f>1/($C2/2.7)*$M2</f>
+        <v>108.18193986525002</v>
+      </c>
+      <c r="E2">
+        <v>2.6179935000000001E-2</v>
+      </c>
+      <c r="F2">
+        <f>(2.7/$E2)*$M2</f>
+        <v>93.757681216550012</v>
+      </c>
+      <c r="G2">
+        <v>2.9670499999999999E-2</v>
+      </c>
+      <c r="H2">
+        <f>2.7/$G2*$M2</f>
+        <v>82.727625082152315</v>
+      </c>
+      <c r="I2">
+        <v>2.4434600000000001E-2</v>
+      </c>
+      <c r="J2">
+        <f>2.7/$I2*$M2</f>
+        <v>100.45468311329017</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE($H2,$D2,$F2,$J2,$B2,$H3,$D3,$F3,$J3,$B3)</f>
+        <v>91.254271275783665</v>
+      </c>
+      <c r="L2">
+        <f>STDEV($D2,$F2,$H2,$J2,$B2,$H3,$D3,$F3,$J3,$B3)</f>
+        <v>12.740353188618007</v>
+      </c>
+      <c r="M2">
+        <v>0.90910000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3">
+        <v>76.2</v>
+      </c>
+      <c r="C3">
+        <v>2.4434600000000001E-2</v>
+      </c>
+      <c r="D3">
+        <f>1/($C3/2.7)*$M3</f>
+        <v>100.54971229322354</v>
+      </c>
+      <c r="E3">
+        <v>2.79253E-2</v>
+      </c>
+      <c r="F3">
+        <f>(2.7/$E3)*$M3</f>
+        <v>87.98086323154989</v>
+      </c>
+      <c r="G3">
+        <v>2.26892E-2</v>
+      </c>
+      <c r="H3">
+        <f>2.7/$G3*$M3</f>
+        <v>108.28464643971581</v>
+      </c>
+      <c r="I3">
+        <v>3.1415822000000003E-2</v>
+      </c>
+      <c r="J3">
+        <f>2.7/$I3*$M3</f>
+        <v>78.205561516104837</v>
+      </c>
+      <c r="M3">
+        <v>0.90995999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4">
+        <v>88.9</v>
+      </c>
+      <c r="C4">
+        <v>1.7453269E-2</v>
+      </c>
+      <c r="D4">
+        <f>1/($C4/2.7)*$M4</f>
+        <v>140.35823317683352</v>
+      </c>
+      <c r="E4">
+        <v>2.4424000000000001E-2</v>
+      </c>
+      <c r="F4">
+        <f>(2.7/$E4)*$M4</f>
+        <v>100.29929577464789</v>
+      </c>
+      <c r="G4">
+        <v>1.3963E-2</v>
+      </c>
+      <c r="H4">
+        <f>2.7/$G4*$M4</f>
+        <v>175.44295638473108</v>
+      </c>
+      <c r="I4">
+        <v>1.9198619E-2</v>
+      </c>
+      <c r="J4">
+        <f>2.7/$I4*$M4</f>
+        <v>127.59824026926104</v>
+      </c>
+      <c r="K4">
+        <f>AVERAGE($H4,$D4,$F4,$J4,$B4)</f>
+        <v>126.51974512109469</v>
+      </c>
+      <c r="L4">
+        <f>STDEV($D4,$F4,$H4,$J4,$B4)</f>
+        <v>34.237788665104965</v>
+      </c>
+      <c r="M4">
+        <v>0.9073</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5">
+        <v>101.6</v>
+      </c>
+      <c r="C5">
+        <v>1.39626E-2</v>
+      </c>
+      <c r="D5">
+        <f>1/($C5/2.7)*$M5</f>
+        <v>161.00296506381332</v>
+      </c>
+      <c r="E5">
+        <v>1.5708125999999999E-2</v>
+      </c>
+      <c r="F5">
+        <f>(2.7/$E5)*$M5</f>
+        <v>143.11191545064003</v>
+      </c>
+      <c r="G5">
+        <v>1.22174E-2</v>
+      </c>
+      <c r="H5">
+        <f>2.7/$G5*$M5</f>
+        <v>184.00150604875017</v>
+      </c>
+      <c r="I5">
+        <v>1.2217E-2</v>
+      </c>
+      <c r="J5">
+        <f>2.7/$I5*$M5</f>
+        <v>184.00753049030041</v>
+      </c>
+      <c r="K5">
+        <f>AVERAGE($H5,$D5,$F5,$J5,$B5,$H6,$D6,$F6,$J6,$B6,$H7,$D7,$F7,$J7,$B7)</f>
+        <v>133.2407471347278</v>
+      </c>
+      <c r="L5">
+        <f>STDEV($D5,$F5,$H5,$J5,$B5,$H6,$D6,$F6,$J6,$B6,$H7,$D7,$F7,$J7,$B7)</f>
+        <v>33.391137641006168</v>
+      </c>
+      <c r="M5">
+        <v>0.83260000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6">
+        <v>101.6</v>
+      </c>
+      <c r="C6">
+        <v>1.9198619E-2</v>
+      </c>
+      <c r="D6">
+        <f>1/($C6/2.7)*$M6</f>
+        <v>128.22547288427361</v>
+      </c>
+      <c r="E6">
+        <v>2.9670592999999999E-2</v>
+      </c>
+      <c r="F6">
+        <f>(2.7/$E6)*$M6</f>
+        <v>82.969423631000581</v>
+      </c>
+      <c r="G6">
+        <v>1.745329E-2</v>
+      </c>
+      <c r="H6">
+        <f>2.7/$G6*$M6</f>
+        <v>141.04802017270097</v>
+      </c>
+      <c r="I6">
+        <v>2.4434606000000001E-2</v>
+      </c>
+      <c r="J6">
+        <f>2.7/$I6*$M6</f>
+        <v>100.74858583764355</v>
+      </c>
+      <c r="M6">
+        <v>0.91176000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7">
+        <v>101.6</v>
+      </c>
+      <c r="C7">
+        <v>2.0943948E-2</v>
+      </c>
+      <c r="D7">
+        <f>1/($C7/2.7)*$M7</f>
+        <v>117.66119740175061</v>
+      </c>
+      <c r="E7">
+        <v>1.5707960999999999E-2</v>
+      </c>
+      <c r="F7">
+        <f>(2.7/$E7)*$M7</f>
+        <v>156.88159653566751</v>
+      </c>
+      <c r="G7">
+        <v>1.3962632000000001E-2</v>
+      </c>
+      <c r="H7">
+        <f>2.7/$G7*$M7</f>
+        <v>176.49179610262593</v>
+      </c>
+      <c r="I7">
+        <v>2.0943948E-2</v>
+      </c>
+      <c r="J7">
+        <f>2.7/$I7*$M7</f>
+        <v>117.66119740175061</v>
+      </c>
+      <c r="M7">
+        <v>0.91269999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8">
+        <v>114.3</v>
+      </c>
+      <c r="C8">
+        <v>1.2217303000000001E-2</v>
+      </c>
+      <c r="D8">
+        <f>1/($C8/2.7)*$M8</f>
+        <v>182.34548165008263</v>
+      </c>
+      <c r="E8">
+        <v>1.0471974E-2</v>
+      </c>
+      <c r="F8">
+        <f>(2.7/$E8)*$M8</f>
+        <v>212.73639525842978</v>
+      </c>
+      <c r="G8">
+        <v>1.2217303000000001E-2</v>
+      </c>
+      <c r="H8">
+        <f>2.7/$G8*$M8</f>
+        <v>182.34548165008266</v>
+      </c>
+      <c r="I8">
+        <v>1.2217303000000001E-2</v>
+      </c>
+      <c r="J8">
+        <f>2.7/$I8*$M8</f>
+        <v>182.34548165008266</v>
+      </c>
+      <c r="K8">
+        <f>AVERAGE($H8,$D8,$F8,$J8,$B8)</f>
+        <v>174.81456804173553</v>
+      </c>
+      <c r="L8">
+        <f>STDEV($D8,$F8,$H8,$J8,$B8)</f>
+        <v>36.29814700525305</v>
+      </c>
+      <c r="M8">
+        <v>0.82509999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>127</v>
+      </c>
+      <c r="C9">
+        <v>8.7266449999999999E-3</v>
+      </c>
+      <c r="D9">
+        <f>1/($C9/2.7)*$M9</f>
+        <v>254.26266337177691</v>
+      </c>
+      <c r="E9">
+        <v>1.0471974E-2</v>
+      </c>
+      <c r="F9">
+        <f>(2.7/$E9)*$M9</f>
+        <v>211.8855528098141</v>
+      </c>
+      <c r="G9">
+        <v>8.7266449999999999E-3</v>
+      </c>
+      <c r="H9">
+        <f>2.7/$G9*$M9</f>
+        <v>254.26266337177691</v>
+      </c>
+      <c r="I9">
+        <v>1.0471974E-2</v>
+      </c>
+      <c r="J9">
+        <f>2.7/$I9*$M9</f>
+        <v>211.8855528098141</v>
+      </c>
+      <c r="K9">
+        <f>AVERAGE($H9,$D9,$F9,$J9,$B9,$H10,$D10,$F10,$J10,$B10)</f>
+        <v>211.02143306677945</v>
+      </c>
+      <c r="L9">
+        <f>STDEV($D9,$F9,$H9,$J9,$B9,$H10,$D10,$F10,$J10,$B10)</f>
+        <v>57.845039203527115</v>
+      </c>
+      <c r="M9">
+        <v>0.82179999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10">
+        <v>127</v>
+      </c>
+      <c r="C10">
+        <v>1.0471974E-2</v>
+      </c>
+      <c r="D10">
+        <f>1/($C10/2.7)*$M10</f>
+        <v>211.80304687540288</v>
+      </c>
+      <c r="E10">
+        <v>6.9813160000000004E-3</v>
+      </c>
+      <c r="F10">
+        <f>(2.7/$E10)*$M10</f>
+        <v>317.70457031310428</v>
+      </c>
+      <c r="G10">
+        <v>1.041974E-2</v>
+      </c>
+      <c r="H10">
+        <f>2.7/$G10*$M10</f>
+        <v>212.8648123657596</v>
+      </c>
+      <c r="I10">
+        <v>1.2217303000000001E-2</v>
+      </c>
+      <c r="J10">
+        <f>2.7/$I10*$M10</f>
+        <v>181.54546875034532</v>
+      </c>
+      <c r="M10">
+        <v>0.82147999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="C11">
+        <v>1.047E-2</v>
+      </c>
+      <c r="D11">
+        <f>1/($C11/2.7)*$M11</f>
+        <v>211.33237822349571</v>
+      </c>
+      <c r="E11">
+        <v>1.2217E-2</v>
+      </c>
+      <c r="F11">
+        <f>(2.7/$E11)*$M11</f>
+        <v>181.11238438241796</v>
+      </c>
+      <c r="G11">
+        <v>1.047E-2</v>
+      </c>
+      <c r="H11">
+        <f>2.7/$G11*$M11</f>
+        <v>211.33237822349571</v>
+      </c>
+      <c r="I11">
+        <v>1.0470999999999999E-2</v>
+      </c>
+      <c r="J11">
+        <f>2.7/$I11*$M11</f>
+        <v>211.31219558781399</v>
+      </c>
+      <c r="K11">
+        <f>AVERAGE($H11,$D11,$F11,$J11,$B11,$H12,$D12,$F12,$J12,$B12)</f>
+        <v>210.90704797615058</v>
+      </c>
+      <c r="L11">
+        <f>STDEV($D11,$F11,$H11,$J11,$B11,$H12,$D12,$F12,$J12,$B12)</f>
+        <v>45.136045245240666</v>
+      </c>
+      <c r="M11">
+        <v>0.81950000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="C12">
+        <v>8.7266449999999999E-3</v>
+      </c>
+      <c r="D12">
+        <f>1/($C12/2.7)*$M12</f>
+        <v>253.64386886369277</v>
+      </c>
+      <c r="E12">
+        <v>8.7264500000000002E-3</v>
+      </c>
+      <c r="F12">
+        <f>(2.7/$E12)*$M12</f>
+        <v>253.64953675320433</v>
+      </c>
+      <c r="G12">
+        <v>8.7266449999999999E-3</v>
+      </c>
+      <c r="H12">
+        <f>2.7/$G12*$M12</f>
+        <v>253.64386886369277</v>
+      </c>
+      <c r="I12">
+        <v>8.7266449999999999E-3</v>
+      </c>
+      <c r="J12">
+        <f>2.7/$I12*$M12</f>
+        <v>253.64386886369277</v>
+      </c>
+      <c r="M12">
+        <v>0.81979999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>50</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B13">
+        <v>177.8</v>
+      </c>
+      <c r="C13">
+        <v>8.7265999999999993E-3</v>
+      </c>
+      <c r="D13">
+        <f>1/($C13/2.7)*$M13</f>
+        <v>270.29083491852504</v>
+      </c>
+      <c r="E13">
+        <v>1.3472899999999999E-2</v>
+      </c>
+      <c r="F13">
+        <f>(2.7/$E13)*$M13</f>
+        <v>175.07143970488912</v>
+      </c>
+      <c r="G13">
+        <v>1.22173E-2</v>
+      </c>
+      <c r="H13">
+        <f>2.7/$G13*$M13</f>
+        <v>193.06393392975536</v>
+      </c>
+      <c r="I13">
+        <v>1.0472E-2</v>
+      </c>
+      <c r="J13">
+        <f>2.7/$I13*$M13</f>
+        <v>225.24064171122996</v>
+      </c>
+      <c r="K13">
+        <f>AVERAGE($H13,$D13,$F13,$J13,$B13)</f>
+        <v>208.29337005287988</v>
+      </c>
+      <c r="L13">
+        <f>STDEV($D13,$F13,$H13,$J13,$B13)</f>
+        <v>39.988666095175681</v>
+      </c>
+      <c r="M13">
+        <v>0.87360000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>51</v>
       </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N1" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2">
-        <v>70</v>
-      </c>
-      <c r="C2">
-        <v>4.8199023199999997</v>
-      </c>
-      <c r="D2">
-        <v>4.3345543339999999</v>
-      </c>
-      <c r="E2">
-        <v>4.4810744810000003</v>
-      </c>
-      <c r="F2">
-        <v>3.9194139190000001</v>
-      </c>
-      <c r="G2">
-        <v>4.7802197800000004</v>
-      </c>
-      <c r="H2">
-        <v>4.3742368740000002</v>
-      </c>
-      <c r="I2">
-        <v>4.6092796089999997</v>
-      </c>
-      <c r="J2">
-        <v>4.0262515260000002</v>
-      </c>
-      <c r="K2">
-        <f>(C2-D2)/(C2+D2)</f>
-        <v>5.301767263138759E-2</v>
-      </c>
-      <c r="L2">
-        <f>(E2-F2)/(E2+F2)</f>
-        <v>6.6860465160573299E-2</v>
-      </c>
-      <c r="M2">
-        <f>(G2-H2)/(G2+H2)</f>
-        <v>4.4348116042759095E-2</v>
-      </c>
-      <c r="N2">
-        <f>(I2-J2)/(I2+J2)</f>
-        <v>6.7515022977217176E-2</v>
-      </c>
-      <c r="P2">
-        <f t="shared" ref="P2:P14" si="0">AVERAGE(K2,L2,M2,N2)</f>
-        <v>5.7935319202984288E-2</v>
-      </c>
-      <c r="Q2">
-        <f>STDEV(K2,L2,M2,N2)</f>
-        <v>1.125794966955484E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3">
-        <v>75</v>
-      </c>
-      <c r="C3">
-        <v>3.5012210010000002</v>
-      </c>
-      <c r="D3">
-        <v>3.2326007319999999</v>
-      </c>
-      <c r="E3">
-        <v>3.5042735039999999</v>
-      </c>
-      <c r="F3">
-        <v>3.2203907200000002</v>
-      </c>
-      <c r="G3">
-        <v>3.5866910860000001</v>
-      </c>
-      <c r="H3">
-        <v>3.217338217</v>
-      </c>
-      <c r="I3">
-        <v>3.3363858359999998</v>
-      </c>
-      <c r="J3">
-        <v>3.0616605610000001</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K14" si="1">(C3-D3)/(C3+D3)</f>
-        <v>3.9891205863616878E-2</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L14" si="2">(E3-F3)/(E3+F3)</f>
-        <v>4.2215161165495209E-2</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M14" si="3">(G3-H3)/(G3+H3)</f>
-        <v>5.4284432437283418E-2</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N14" si="4">(I3-J3)/(I3+J3)</f>
-        <v>4.2938931347671468E-2</v>
-      </c>
-      <c r="P3">
-        <f t="shared" si="0"/>
-        <v>4.4832432703516743E-2</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q14" si="5">STDEV(K3,L3,M3,N3)</f>
-        <v>6.4340624631409353E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4">
-        <v>35</v>
-      </c>
-      <c r="C4">
-        <v>1.819291819</v>
-      </c>
-      <c r="D4">
-        <v>1.599511599</v>
-      </c>
-      <c r="E4">
-        <v>1.78261783</v>
-      </c>
-      <c r="F4">
-        <v>1.2789987789999999</v>
-      </c>
-      <c r="G4">
-        <v>1.3003663000000001</v>
-      </c>
-      <c r="H4">
-        <v>0.84249084200000002</v>
-      </c>
-      <c r="I4">
-        <v>1.568986569</v>
-      </c>
-      <c r="J4">
-        <v>1.1080586079999999</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="1"/>
-        <v>6.4285714365107161E-2</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="2"/>
-        <v>0.16449448618731349</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="3"/>
-        <v>0.21367521381880344</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="4"/>
-        <v>0.17217787916322494</v>
-      </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
-        <v>0.15365832338361227</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" si="5"/>
-        <v>6.3376879987544377E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5">
-        <v>30</v>
-      </c>
-      <c r="C5">
-        <v>1.993284493</v>
-      </c>
-      <c r="D5">
-        <v>1.7338217339999999</v>
-      </c>
-      <c r="E5">
-        <v>1.886446887</v>
-      </c>
-      <c r="F5">
-        <v>1.1385836389999999</v>
-      </c>
-      <c r="G5">
-        <v>1.7155067159999999</v>
-      </c>
-      <c r="H5">
-        <v>0.98595848600000002</v>
-      </c>
-      <c r="I5">
-        <v>1.0073260070000001</v>
-      </c>
-      <c r="J5">
-        <v>0.57081807100000004</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="1"/>
-        <v>6.9615069492893214E-2</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="2"/>
-        <v>0.2472250251930185</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="3"/>
-        <v>0.27005649728891079</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="4"/>
-        <v>0.27659574438424628</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
-        <v>0.21587308408976721</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="5"/>
-        <v>9.8314859480326311E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-      <c r="C6">
-        <v>2.1031746029999998</v>
-      </c>
-      <c r="D6">
-        <v>1.849816849</v>
-      </c>
-      <c r="E6">
-        <v>1.9108669110000001</v>
-      </c>
-      <c r="F6">
-        <v>1.1782661780000001</v>
-      </c>
-      <c r="G6">
-        <v>1.9291819290000001</v>
-      </c>
-      <c r="H6">
-        <v>1.123321123</v>
-      </c>
-      <c r="I6">
-        <v>1.2057387049999999</v>
-      </c>
-      <c r="J6">
-        <v>0.66849846800000001</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>6.4092664271210228E-2</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="2"/>
-        <v>0.23715415033709475</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="3"/>
-        <v>0.26400000008910723</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="4"/>
-        <v>0.28664474525391342</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
-        <v>0.21297288998783143</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="5"/>
-        <v>0.10129390107527893</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7">
-        <v>40</v>
-      </c>
-      <c r="C7">
-        <v>2.0054945050000001</v>
-      </c>
-      <c r="D7">
-        <v>1.6025641020000001</v>
-      </c>
-      <c r="E7">
-        <v>1.6239316239999999</v>
-      </c>
-      <c r="F7">
-        <v>1.184371184</v>
-      </c>
-      <c r="G7">
-        <v>1.1874236869999999</v>
-      </c>
-      <c r="H7">
-        <v>0.70512820499999995</v>
-      </c>
-      <c r="I7">
-        <v>1.053113553</v>
-      </c>
-      <c r="J7">
-        <v>0.61965811900000001</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
-        <v>0.11167512695560824</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="2"/>
-        <v>0.15652173930383365</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="3"/>
-        <v>0.25483870959560456</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="4"/>
-        <v>0.25912408803632581</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
-        <v>0.19553991597284306</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="5"/>
-        <v>7.3291688500112945E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8">
-        <v>40</v>
-      </c>
-      <c r="C8">
-        <v>1.6758241760000001</v>
-      </c>
-      <c r="D8">
-        <v>1.367521368</v>
-      </c>
-      <c r="E8">
-        <v>1.404151404</v>
-      </c>
-      <c r="F8">
-        <v>1.040903541</v>
-      </c>
-      <c r="G8">
-        <v>1.101953602</v>
-      </c>
-      <c r="H8">
-        <v>0.65628815699999998</v>
-      </c>
-      <c r="I8">
-        <v>1.1202686209999999</v>
-      </c>
-      <c r="J8">
-        <v>0.83943833999999995</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
-        <v>0.10130391161392223</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="2"/>
-        <v>0.14856429453367562</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="3"/>
-        <v>0.25347222173444012</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="4"/>
-        <v>0.14330218067740996</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>0.16166065213986197</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="5"/>
-        <v>6.4758135898954766E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9">
-        <v>55</v>
-      </c>
-      <c r="C9">
-        <v>1.1141636150000001</v>
-      </c>
-      <c r="D9">
-        <v>0.86691086699999997</v>
-      </c>
-      <c r="E9">
-        <v>1.11111111</v>
-      </c>
-      <c r="F9">
-        <v>0.85164835299999997</v>
-      </c>
-      <c r="G9">
-        <v>0.99816849900000004</v>
-      </c>
-      <c r="H9">
-        <v>0.65018315100000001</v>
-      </c>
-      <c r="I9">
-        <v>0.958485959</v>
-      </c>
-      <c r="J9">
-        <v>0.69597069600000006</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
-        <v>0.12480739631272485</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="2"/>
-        <v>0.13219284476327092</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="3"/>
-        <v>0.2111111109088889</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="4"/>
-        <v>0.15867158695674619</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>0.15669573473540771</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="5"/>
-        <v>3.9081943402924695E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10">
-        <v>55</v>
-      </c>
-      <c r="C10">
-        <v>1.043956044</v>
-      </c>
-      <c r="D10">
-        <v>0.89133089200000004</v>
-      </c>
-      <c r="E10">
-        <v>0.99206349199999999</v>
-      </c>
-      <c r="F10">
-        <v>0.71733821799999997</v>
-      </c>
-      <c r="G10">
-        <v>0.753968254</v>
-      </c>
-      <c r="H10">
-        <v>0.497557998</v>
-      </c>
-      <c r="I10">
-        <v>0.57692307700000001</v>
-      </c>
-      <c r="J10">
-        <v>0.27472527499999999</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>7.8864352960216502E-2</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="2"/>
-        <v>0.16071428523375003</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="3"/>
-        <v>0.20487804837512907</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="4"/>
-        <v>0.35483870929864725</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="0"/>
-        <v>0.19982384896693572</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="5"/>
-        <v>0.11578127296029272</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11">
-        <v>50</v>
-      </c>
-      <c r="C11">
-        <v>1.3614163619999999</v>
-      </c>
-      <c r="D11">
-        <v>1.083638584</v>
-      </c>
-      <c r="E11">
-        <v>1.2515262519999999</v>
-      </c>
-      <c r="F11">
-        <v>0.8241175825</v>
-      </c>
-      <c r="G11">
-        <v>0.92796092799999996</v>
-      </c>
-      <c r="H11">
-        <v>0.45787545800000001</v>
-      </c>
-      <c r="I11">
-        <v>0.55555555555000002</v>
-      </c>
-      <c r="J11">
-        <v>0.20451770499999999</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="1"/>
-        <v>0.11360799005945935</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="2"/>
-        <v>0.20591618966408945</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="3"/>
-        <v>0.3392070483564284</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="4"/>
-        <v>0.46184738862670155</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="0"/>
-        <v>0.28014465417666967</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="5"/>
-        <v>0.15247794982887197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12">
-        <v>50</v>
-      </c>
-      <c r="C12">
-        <v>1.324786325</v>
-      </c>
-      <c r="D12">
-        <v>1.0103785110000001</v>
-      </c>
-      <c r="E12">
-        <v>1.2087912089999999</v>
-      </c>
-      <c r="F12">
-        <v>0.87912087999999999</v>
-      </c>
-      <c r="G12">
-        <v>1.0195360200000001</v>
-      </c>
-      <c r="H12">
-        <v>0.69902319899999998</v>
-      </c>
-      <c r="I12">
-        <v>0.79975580000000002</v>
-      </c>
-      <c r="J12">
-        <v>0.45787545800000001</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="1"/>
-        <v>0.13464052265302265</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="2"/>
-        <v>0.15789473643878113</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="3"/>
-        <v>0.18650088833511422</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="4"/>
-        <v>0.27184466020961451</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="0"/>
-        <v>0.18772020190913313</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="5"/>
-        <v>5.9959491743442693E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13">
-        <v>45</v>
-      </c>
-      <c r="C13">
-        <v>1.1996336990000001</v>
-      </c>
-      <c r="D13">
-        <v>0.97985347899999997</v>
-      </c>
-      <c r="E13">
-        <v>1.1446886439999999</v>
-      </c>
-      <c r="F13">
-        <v>0.79059829000000004</v>
-      </c>
-      <c r="G13">
-        <v>0.98290598299999998</v>
-      </c>
-      <c r="H13">
-        <v>0.57692307700000001</v>
-      </c>
-      <c r="I13">
-        <v>0.75091575099999996</v>
-      </c>
-      <c r="J13">
-        <v>0.363247863</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="1"/>
-        <v>0.10084033630410286</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="2"/>
-        <v>0.18296529975952386</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="3"/>
-        <v>0.26027397258517543</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="4"/>
-        <v>0.34794520582862976</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="0"/>
-        <v>0.223006203619358</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="5"/>
-        <v>0.10571410185895873</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>76</v>
-      </c>
       <c r="B14">
-        <v>40</v>
+        <v>190.5</v>
       </c>
       <c r="C14">
-        <v>2.2649572650000001</v>
+        <v>5.1399999999999996E-3</v>
       </c>
       <c r="D14">
-        <v>1.6971916970000001</v>
+        <f>1/($C14/2.7)*$M14</f>
+        <v>475.5992217898833</v>
       </c>
       <c r="E14">
-        <v>2.133699633</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="F14">
-        <v>1.468253968</v>
+        <f>(2.7/$E14)*$M14</f>
+        <v>349.22571428571428</v>
       </c>
       <c r="G14">
-        <v>1.813186813</v>
+        <v>5.2329999999999998E-3</v>
       </c>
       <c r="H14">
-        <v>1.245421245</v>
+        <f>2.7/$G14*$M14</f>
+        <v>467.14695203516146</v>
       </c>
       <c r="I14">
-        <v>1.434676434</v>
+        <v>5.2337E-3</v>
       </c>
       <c r="J14">
-        <v>0.87912087900000002</v>
+        <f>2.7/$I14*$M14</f>
+        <v>467.08447178860087</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
-        <v>0.14329738065007158</v>
+        <f>AVERAGE($H14,$D14,$F14,$J14,$B14)</f>
+        <v>389.91127197987197</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
-        <v>0.18474576263704626</v>
+        <f>STDEV($D14,$F14,$H14,$J14,$B14)</f>
+        <v>123.17025592901788</v>
       </c>
       <c r="M14">
-        <f t="shared" si="3"/>
-        <v>0.18562874262852022</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="4"/>
-        <v>0.24010554073973026</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="0"/>
-        <v>0.18844435666384207</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="5"/>
-        <v>3.9701950680378947E-2</v>
+        <v>0.90539999999999998</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:M14">
+    <sortCondition ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2223,8 +3002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2234,10 +3013,10 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2388,5 +3167,6 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>